<commit_message>
Add files for routing vagus trunks
</commit_message>
<xml_diff>
--- a/visualisation/Organs/organ_provenance.xlsx
+++ b/visualisation/Organs/organ_provenance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlin865\manInBox\nerveImprovements\visualisation\Organs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C470255B-9CD9-47B7-9584-25C0CCDD2FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C825024-CC9C-43B6-8CE4-12DD911B8AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>File</t>
   </si>
@@ -33,39 +33,12 @@
     <t>Origin</t>
   </si>
   <si>
-    <t>bones.exf</t>
-  </si>
-  <si>
     <t>Geometry_Fitter_Wholebody.exf</t>
   </si>
   <si>
-    <t>Left scapula.exf</t>
-  </si>
-  <si>
-    <t>left_clavicle.exf</t>
-  </si>
-  <si>
-    <t>muscles.exf</t>
-  </si>
-  <si>
-    <t>Right scapula.exf</t>
-  </si>
-  <si>
-    <t>right_clavicle.exf</t>
-  </si>
-  <si>
-    <t>vertebral column.exf</t>
-  </si>
-  <si>
     <t>https://sparc.science/datasets/file/307/6?path=files/primary/mapclient_workflow/Organs/Geometry_Fitter_Wholebody.exf</t>
   </si>
   <si>
-    <t>https://sparc.science/datasets/file/307/6?path=files/primary/mapclient_workflow/Organs/bones.exf</t>
-  </si>
-  <si>
-    <t>https://sparc.science/datasets/file/307/6?path=files/primary/mapclient_workflow/Organs/muscles.exf</t>
-  </si>
-  <si>
     <t>converted to exf from obj extracted from https://lifesciencedb.jp/bp3d/</t>
   </si>
   <si>
@@ -93,9 +66,6 @@
     <t>https://sparc.science/datasets/file/307/6?path=files/primary/mapclient_workflow/Organs/lung.exf</t>
   </si>
   <si>
-    <t>https://sparc.science/datasets/file/307/6?path=files/primary/mapclient_workflow/Organs/nervesWithVagus.exf</t>
-  </si>
-  <si>
     <t>https://sparc.science/datasets/file/307/6?path=files/primary/mapclient_workflow/Organs/heart.exf</t>
   </si>
   <si>
@@ -103,13 +73,31 @@
   </si>
   <si>
     <t>https://sparc.science/datasets/file/307/6?path=files/primary/mapclient_workflow/Organs/arteries.exf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://sparc.science/datasets/file/307/6?path=files/primary/mapclient_workflow/Organs/nervesWithVagus.exf  </t>
+  </si>
+  <si>
+    <t>veins.exf</t>
+  </si>
+  <si>
+    <t>https://sparc.science/datasets/file/307/6?path=files/primary/mapclient_workflow/Organs/veins.exf</t>
+  </si>
+  <si>
+    <t>manubrium.exf</t>
+  </si>
+  <si>
+    <t>brainstem.exf</t>
+  </si>
+  <si>
+    <t>https://sparc.science/datasets/file/307/6?path=files/primary/mapclient_workflow/Organs/brainstem.exf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +109,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -143,14 +139,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -429,7 +428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -453,12 +452,12 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -466,101 +465,72 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
         <v>4</v>
       </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{16E32045-634C-4C4D-BF55-042926AC4CFB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>